<commit_message>
added 18-19 K_B numbers to initial state vectors
</commit_message>
<xml_diff>
--- a/Initial_state_vector_&_transition_probability_parameters.xlsx
+++ b/Initial_state_vector_&_transition_probability_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IQBIO\Rotation 1\BVSD-GT-Research-New\BVSD-GT-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5317AAA2-7DC8-4DD1-9B85-575A4457F3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBF05FA-DF6B-46E0-A7E2-7910F3451B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1990,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77:D89"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2020,7 +2020,7 @@
         <v>52</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -2185,7 +2185,7 @@
         <v>67</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -2350,7 +2350,7 @@
         <v>83</v>
       </c>
       <c r="C32" s="1">
-        <v>0</v>
+        <v>369</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -2515,7 +2515,7 @@
         <v>97</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -2680,7 +2680,7 @@
         <v>112</v>
       </c>
       <c r="C62" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
started to add K_B values for other years
</commit_message>
<xml_diff>
--- a/Initial_state_vector_&_transition_probability_parameters.xlsx
+++ b/Initial_state_vector_&_transition_probability_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IQBIO\Rotation 1\BVSD-GT-Research-New\BVSD-GT-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBF05FA-DF6B-46E0-A7E2-7910F3451B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F11BF4-5CFB-4171-828B-13022A246593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="365">
   <si>
     <t>Beta_0_Yr_1_W</t>
   </si>
@@ -1125,6 +1125,9 @@
   </si>
   <si>
     <t>Other yr4</t>
+  </si>
+  <si>
+    <t>K_B</t>
   </si>
 </sst>
 </file>
@@ -1988,10 +1991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C336"/>
+  <dimension ref="A1:C375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="A338" sqref="A338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5956,6 +5959,127 @@
         <v>0</v>
       </c>
     </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A337" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A338" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A339" s="5"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A340" s="5"/>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A341" s="5"/>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A342" s="5"/>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A343" s="5"/>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A344" s="5"/>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A345" s="5"/>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A346" s="5"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A347" s="5"/>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A348" s="5"/>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A349" s="5"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A350" s="5"/>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A351" s="5"/>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A352" s="5"/>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A353" s="5"/>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A354" s="5"/>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A355" s="5"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A356" s="5"/>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A357" s="5"/>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A358" s="5"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A359" s="5"/>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A360" s="5"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A361" s="5"/>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A362" s="5"/>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A363" s="5"/>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A364" s="5"/>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A365" s="5"/>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A366" s="5"/>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A367" s="5"/>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A368" s="5"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A369" s="5"/>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A370" s="5"/>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A371" s="5"/>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A372" s="5"/>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A373" s="5"/>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A374" s="5"/>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A375" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished adding K_B values for all races and years
</commit_message>
<xml_diff>
--- a/Initial_state_vector_&_transition_probability_parameters.xlsx
+++ b/Initial_state_vector_&_transition_probability_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IQBIO\Rotation 1\BVSD-GT-Research-New\BVSD-GT-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F11BF4-5CFB-4171-828B-13022A246593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CD8DCC-85F9-4F64-8CD8-EF309F7B25AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="379">
   <si>
     <t>Beta_0_Yr_1_W</t>
   </si>
@@ -1127,7 +1127,49 @@
     <t>Other yr4</t>
   </si>
   <si>
-    <t>K_B</t>
+    <t>White yr2 K_B</t>
+  </si>
+  <si>
+    <t>Asian yr2 K_B</t>
+  </si>
+  <si>
+    <t>Latinx yr2 K_B</t>
+  </si>
+  <si>
+    <t>2MR yr2 K_B</t>
+  </si>
+  <si>
+    <t>Other yr2 K_B</t>
+  </si>
+  <si>
+    <t>White yr3 K_B</t>
+  </si>
+  <si>
+    <t>Asian yr3 K_B</t>
+  </si>
+  <si>
+    <t>Latinx yr3 K_B</t>
+  </si>
+  <si>
+    <t>2MR yr3 K_B</t>
+  </si>
+  <si>
+    <t>Other yr3 K_B</t>
+  </si>
+  <si>
+    <t>White yr4 K_B</t>
+  </si>
+  <si>
+    <t>Asian yr4 K_B</t>
+  </si>
+  <si>
+    <t>Latinx yr4 K_B</t>
+  </si>
+  <si>
+    <t>2MR yr4 K_B</t>
+  </si>
+  <si>
+    <t>Other yr4 K_B</t>
   </si>
 </sst>
 </file>
@@ -1993,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
-      <selection activeCell="A338" sqref="A338"/>
+    <sheetView tabSelected="1" topLeftCell="A328" workbookViewId="0">
+      <selection activeCell="G341" sqref="G341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5959,56 +6001,127 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A337" s="5" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C337">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A338" s="5" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A339" s="5"/>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A340" s="5"/>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A341" s="5"/>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A342" s="5"/>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A343" s="5"/>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A344" s="5"/>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A345" s="5"/>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A346" s="5"/>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A347" s="5"/>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A348" s="5"/>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A349" s="5"/>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A350" s="5"/>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A351" s="5"/>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.45">
+        <v>365</v>
+      </c>
+      <c r="C338">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A339" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C339">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A340" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C340">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A341" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C341">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A342" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C342">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A343" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C343">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A344" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C344">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A345" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C345">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A346" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C346">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A347" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C347">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A348" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C348">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A349" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C349">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A350" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C350">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A351" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="C351">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A352" s="5"/>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.45">

</xml_diff>